<commit_message>
Refined instructions, added dependency injection
</commit_message>
<xml_diff>
--- a/Instructions.xlsx
+++ b/Instructions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eckst\Desktop\Git Projects\MiniPC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8F100E9-E1D8-4D8E-BFF9-597371AF5C1D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F36B93E1-EF23-4202-B591-4700F86372E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28800" yWindow="16200" windowWidth="28800" windowHeight="15600" xr2:uid="{61453D25-6AEE-443B-8D59-9EA4C4B044E4}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="181">
   <si>
     <t>Nmonic</t>
   </si>
@@ -114,9 +114,6 @@
     <t>Store through register</t>
   </si>
   <si>
-    <t>MOV</t>
-  </si>
-  <si>
     <t>Copy contents of another register</t>
   </si>
   <si>
@@ -375,9 +372,6 @@
     <t>SPC</t>
   </si>
   <si>
-    <t>PSH</t>
-  </si>
-  <si>
     <t>Push contents onto stack</t>
   </si>
   <si>
@@ -568,6 +562,21 @@
   </si>
   <si>
     <t>0011_11</t>
+  </si>
+  <si>
+    <t>Return to normal processing from interrupt</t>
+  </si>
+  <si>
+    <t>PUSH</t>
+  </si>
+  <si>
+    <t>MOVE</t>
+  </si>
+  <si>
+    <t>RTIN</t>
+  </si>
+  <si>
+    <t>HALT</t>
   </si>
 </sst>
 </file>
@@ -950,7 +959,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD869FDA-EC45-4E05-88AC-2BBE8F223278}">
   <dimension ref="A1:E65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -976,15 +987,18 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="B2" s="2" t="s">
+        <v>180</v>
+      </c>
       <c r="C2" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>3</v>
@@ -998,13 +1012,13 @@
         <v>20</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>17</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1013,13 +1027,13 @@
         <v>21</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>18</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1028,13 +1042,13 @@
         <v>22</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>19</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1045,13 +1059,13 @@
         <v>8</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1060,13 +1074,13 @@
         <v>10</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1075,13 +1089,13 @@
         <v>11</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1090,13 +1104,13 @@
         <v>13</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1104,333 +1118,333 @@
         <v>15</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>68</v>
-      </c>
       <c r="E10" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>66</v>
-      </c>
       <c r="E11" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="D12" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>101</v>
-      </c>
       <c r="E12" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C13" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C14" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>104</v>
-      </c>
       <c r="E14" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="D15" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>107</v>
-      </c>
       <c r="E15" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C16" s="2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C17" s="2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C18" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="E18" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>33</v>
-      </c>
       <c r="E19" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C20" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>35</v>
-      </c>
       <c r="E20" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C21" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>38</v>
-      </c>
       <c r="E21" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C24" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>43</v>
-      </c>
       <c r="E24" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="B26" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D26" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C26" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>46</v>
-      </c>
       <c r="E26" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
       <c r="B27" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D27" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C27" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>48</v>
-      </c>
       <c r="E27" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
       <c r="B28" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D28" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C28" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>50</v>
-      </c>
       <c r="E28" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
       <c r="B29" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D29" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C29" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>52</v>
-      </c>
       <c r="E29" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
       <c r="B30" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D30" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C30" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>54</v>
-      </c>
       <c r="E30" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="3"/>
       <c r="B31" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D31" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C31" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>56</v>
-      </c>
       <c r="E31" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="3"/>
       <c r="B32" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D32" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C32" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>58</v>
-      </c>
       <c r="E32" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="3"/>
       <c r="B33" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D33" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C33" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>60</v>
-      </c>
       <c r="E33" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -1438,245 +1452,251 @@
         <v>23</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
       <c r="B35" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>24</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
       <c r="B36" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
       <c r="B37" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>25</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C38" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C39" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C40" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C41" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C42" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C43" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C44" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C45" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C46" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C47" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C48" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C49" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>113</v>
+        <v>177</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="3"/>
       <c r="B51" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C52" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C53" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C54" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C55" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C56" s="2" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C57" s="2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B58" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D58" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C58" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="D58" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="E58" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="4"/>
       <c r="B59" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B60" s="2" t="s">
+        <v>179</v>
+      </c>
       <c r="C60" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C61" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C62" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C63" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C64" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="65" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C65" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -1703,79 +1723,79 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Started creating processor instructions
</commit_message>
<xml_diff>
--- a/Instructions.xlsx
+++ b/Instructions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eckst\Desktop\Git Projects\MiniPC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F36B93E1-EF23-4202-B591-4700F86372E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E27DDED8-6F21-4B85-B139-B78876F9099E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="16200" windowWidth="28800" windowHeight="15600" xr2:uid="{61453D25-6AEE-443B-8D59-9EA4C4B044E4}"/>
+    <workbookView xWindow="28800" yWindow="0" windowWidth="28800" windowHeight="31800" xr2:uid="{61453D25-6AEE-443B-8D59-9EA4C4B044E4}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -959,8 +959,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD869FDA-EC45-4E05-88AC-2BBE8F223278}">
   <dimension ref="A1:E65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1018,7 +1018,7 @@
         <v>17</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1033,7 +1033,7 @@
         <v>18</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1048,7 +1048,7 @@
         <v>19</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1194,7 +1194,7 @@
         <v>106</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>143</v>
+        <v>128</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>